<commit_message>
Spring 2017 Semster Over
</commit_message>
<xml_diff>
--- a/Docs/march-madness-bracket.xlsx
+++ b/Docs/march-madness-bracket.xlsx
@@ -4483,8 +4483,8 @@
   </sheetPr>
   <dimension ref="A1:AJ70"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52:S53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4872,7 +4872,9 @@
         <f>IF(F6&gt;F10,E6,IF(F10&gt;F6,E10,""))</f>
         <v>Wisconsin</v>
       </c>
-      <c r="H8" s="151"/>
+      <c r="H8" s="151">
+        <v>1</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="6"/>
       <c r="K8" s="1"/>
@@ -4887,7 +4889,9 @@
       <c r="T8" s="1"/>
       <c r="U8" s="6"/>
       <c r="V8" s="1"/>
-      <c r="W8" s="151"/>
+      <c r="W8" s="151">
+        <v>98</v>
+      </c>
       <c r="X8" s="153" t="str">
         <f>IF(Y10&gt;Y6,Z10,IF(Y6&gt;Y10,Z6,""))</f>
         <v>Kansas</v>
@@ -5054,9 +5058,11 @@
       <c r="H12" s="26"/>
       <c r="I12" s="147" t="str">
         <f>IF(H8&gt;H16,G8,IF(H16&gt;H8,G16,""))</f>
-        <v/>
-      </c>
-      <c r="J12" s="151"/>
+        <v>Florida</v>
+      </c>
+      <c r="J12" s="151">
+        <v>1</v>
+      </c>
       <c r="K12" s="1"/>
       <c r="L12" s="6"/>
       <c r="M12" s="1"/>
@@ -5067,10 +5073,12 @@
       <c r="R12" s="1"/>
       <c r="S12" s="6"/>
       <c r="T12" s="1"/>
-      <c r="U12" s="151"/>
+      <c r="U12" s="151">
+        <v>1</v>
+      </c>
       <c r="V12" s="153" t="str">
         <f>IF(W16&gt;W8,X16,IF(W8&gt;W16,X8,""))</f>
-        <v/>
+        <v>Kansas</v>
       </c>
       <c r="W12" s="27"/>
       <c r="X12" s="156" t="str">
@@ -5241,7 +5249,9 @@
         <f>IF(F14&gt;F18,E14,IF(F18&gt;F14,E18,""))</f>
         <v>Florida</v>
       </c>
-      <c r="H16" s="149"/>
+      <c r="H16" s="149">
+        <v>2</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="26"/>
       <c r="K16" s="1"/>
@@ -5256,7 +5266,9 @@
       <c r="T16" s="1"/>
       <c r="U16" s="27"/>
       <c r="V16" s="1"/>
-      <c r="W16" s="159"/>
+      <c r="W16" s="159">
+        <v>66</v>
+      </c>
       <c r="X16" s="153" t="str">
         <f>IF(Y18&gt;Y14,Z18,IF(Y14&gt;Y18,Z14,""))</f>
         <v>Purdue</v>
@@ -5424,7 +5436,7 @@
       <c r="J20" s="26"/>
       <c r="K20" s="147" t="str">
         <f>IF(J12&gt;J28,I12,IF(J28&gt;J12,I28,""))</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="L20" s="151"/>
       <c r="M20" s="1"/>
@@ -5436,7 +5448,7 @@
       <c r="S20" s="151"/>
       <c r="T20" s="153" t="str">
         <f>IF(U28&gt;U12,V28,IF(U12&gt;U28,V12,""))</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="U20" s="27"/>
       <c r="V20" s="158" t="s">
@@ -5613,7 +5625,9 @@
         <f>IF(F22&gt;F26,E22,IF(F26&gt;F22,E26,""))</f>
         <v>Baylor</v>
       </c>
-      <c r="H24" s="151"/>
+      <c r="H24" s="151">
+        <v>1</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="26"/>
       <c r="K24" s="1"/>
@@ -5628,7 +5642,9 @@
       <c r="T24" s="1"/>
       <c r="U24" s="27"/>
       <c r="V24" s="1"/>
-      <c r="W24" s="151"/>
+      <c r="W24" s="151">
+        <v>69</v>
+      </c>
       <c r="X24" s="153" t="str">
         <f>IF(Y26&gt;Y22,Z26,IF(Y22&gt;Y26,Z22,""))</f>
         <v>Oregon</v>
@@ -5795,9 +5811,11 @@
       <c r="H28" s="26"/>
       <c r="I28" s="147" t="str">
         <f>IF(H24&gt;H32,G24,IF(H32&gt;H24,G32,""))</f>
-        <v/>
-      </c>
-      <c r="J28" s="149"/>
+        <v>South Carolina</v>
+      </c>
+      <c r="J28" s="149">
+        <v>2</v>
+      </c>
       <c r="K28" s="1"/>
       <c r="L28" s="26"/>
       <c r="M28" s="147" t="str">
@@ -5811,10 +5829,12 @@
       <c r="R28" s="1"/>
       <c r="S28" s="27"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="159"/>
+      <c r="U28" s="159">
+        <v>2</v>
+      </c>
       <c r="V28" s="153" t="str">
         <f>IF(W32&gt;W24,X32,IF(W24&gt;W32,X24,""))</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="W28" s="27"/>
       <c r="X28" s="156" t="str">
@@ -5983,7 +6003,9 @@
         <f>IF(F30&gt;F34,E30,IF(F34&gt;F30,E34,""))</f>
         <v>South Carolina</v>
       </c>
-      <c r="H32" s="149"/>
+      <c r="H32" s="149">
+        <v>2</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="6"/>
       <c r="K32" s="1"/>
@@ -6000,7 +6022,9 @@
       <c r="T32" s="1"/>
       <c r="U32" s="6"/>
       <c r="V32" s="1"/>
-      <c r="W32" s="159"/>
+      <c r="W32" s="159">
+        <v>68</v>
+      </c>
       <c r="X32" s="153" t="str">
         <f>IF(Y34&gt;Y30,Z34,IF(Y30&gt;Y34,Z30,""))</f>
         <v>Michigan</v>
@@ -6354,7 +6378,9 @@
         <f>IF(F38&gt;F42,E38,IF(F42&gt;F38,E42,""))</f>
         <v>Gonzaga</v>
       </c>
-      <c r="H40" s="151"/>
+      <c r="H40" s="151">
+        <v>61</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="6"/>
       <c r="K40" s="34"/>
@@ -6372,7 +6398,9 @@
       <c r="T40" s="1"/>
       <c r="U40" s="6"/>
       <c r="V40" s="1"/>
-      <c r="W40" s="151"/>
+      <c r="W40" s="151">
+        <v>2</v>
+      </c>
       <c r="X40" s="153" t="str">
         <f>IF(Y42&gt;Y38,Z42,IF(Y38&gt;Y42,Z38,""))</f>
         <v>North Carolina</v>
@@ -6537,9 +6565,11 @@
       <c r="H44" s="26"/>
       <c r="I44" s="147" t="str">
         <f>IF(H40&gt;H48,G40,IF(H48&gt;H40,G48,""))</f>
-        <v/>
-      </c>
-      <c r="J44" s="151"/>
+        <v>Gonzaga</v>
+      </c>
+      <c r="J44" s="151">
+        <v>2</v>
+      </c>
       <c r="K44" s="34"/>
       <c r="L44" s="26"/>
       <c r="M44" s="1"/>
@@ -6550,10 +6580,12 @@
       <c r="R44" s="1"/>
       <c r="S44" s="27"/>
       <c r="T44" s="1"/>
-      <c r="U44" s="151"/>
+      <c r="U44" s="151">
+        <v>3</v>
+      </c>
       <c r="V44" s="153" t="str">
         <f>IF(W48&gt;W40,X48,IF(W40&gt;W48,X40,""))</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="W44" s="27"/>
       <c r="X44" s="156" t="str">
@@ -6717,7 +6749,9 @@
         <f>IF(F46&gt;F50,E46,IF(F50&gt;F46,E50,""))</f>
         <v>West Virginia</v>
       </c>
-      <c r="H48" s="149"/>
+      <c r="H48" s="149">
+        <v>58</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="26"/>
       <c r="K48" s="34"/>
@@ -6732,7 +6766,9 @@
       <c r="T48" s="1"/>
       <c r="U48" s="27"/>
       <c r="V48" s="1"/>
-      <c r="W48" s="159"/>
+      <c r="W48" s="159">
+        <v>1</v>
+      </c>
       <c r="X48" s="153" t="str">
         <f>IF(Y50&gt;Y46,Z50,IF(Y46&gt;Y50,Z46,""))</f>
         <v>Butler</v>
@@ -6898,7 +6934,7 @@
       <c r="J52" s="26"/>
       <c r="K52" s="147" t="str">
         <f>IF(J44&gt;J60,I44,IF(J60&gt;J44,I60,""))</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="L52" s="149"/>
       <c r="M52" s="1"/>
@@ -6910,7 +6946,7 @@
       <c r="S52" s="159"/>
       <c r="T52" s="153" t="str">
         <f>IF(U60&gt;U44,V60,IF(U44&gt;U60,V44,""))</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="U52" s="27"/>
       <c r="V52" s="158" t="s">
@@ -7005,7 +7041,9 @@
       </c>
       <c r="W54" s="6"/>
       <c r="X54" s="6"/>
-      <c r="Y54" s="151"/>
+      <c r="Y54" s="151">
+        <v>1</v>
+      </c>
       <c r="Z54" s="153" t="str">
         <f>IF(AA56&gt;AA54,AB56,IF(AA54&gt;AA56,AB54,""))</f>
         <v>Cincinnati</v>
@@ -7079,7 +7117,9 @@
         <f>IF(F54&gt;F58,E54,IF(F58&gt;F54,E58,""))</f>
         <v>Xavier</v>
       </c>
-      <c r="H56" s="151"/>
+      <c r="H56" s="151">
+        <v>73</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="26"/>
       <c r="K56" s="1"/>
@@ -7094,10 +7134,12 @@
       <c r="T56" s="1"/>
       <c r="U56" s="27"/>
       <c r="V56" s="1"/>
-      <c r="W56" s="151"/>
+      <c r="W56" s="151">
+        <v>1</v>
+      </c>
       <c r="X56" s="153" t="str">
         <f>IF(Y58&gt;Y54,Z58,IF(Y54&gt;Y58,Z54,""))</f>
-        <v/>
+        <v>UCLA</v>
       </c>
       <c r="Y56" s="25"/>
       <c r="Z56" s="155" t="str">
@@ -7183,7 +7225,9 @@
       <c r="V58" s="1"/>
       <c r="W58" s="25"/>
       <c r="X58" s="6"/>
-      <c r="Y58" s="159"/>
+      <c r="Y58" s="159">
+        <v>2</v>
+      </c>
       <c r="Z58" s="153" t="str">
         <f>IF(AA60&gt;AA58,AB60,IF(AA58&gt;AA60,AB58,""))</f>
         <v>UCLA</v>
@@ -7257,9 +7301,11 @@
       <c r="H60" s="26"/>
       <c r="I60" s="147" t="str">
         <f>IF(H56&gt;H64,G56,IF(H64&gt;H56,G64,""))</f>
-        <v/>
-      </c>
-      <c r="J60" s="149"/>
+        <v>Xavier</v>
+      </c>
+      <c r="J60" s="149">
+        <v>1</v>
+      </c>
       <c r="K60" s="1"/>
       <c r="L60" s="2"/>
       <c r="M60" s="1"/>
@@ -7270,10 +7316,12 @@
       <c r="R60" s="1"/>
       <c r="S60" s="6"/>
       <c r="T60" s="1"/>
-      <c r="U60" s="159"/>
+      <c r="U60" s="159">
+        <v>2</v>
+      </c>
       <c r="V60" s="153" t="str">
         <f>IF(W64&gt;W56,X64,IF(W56&gt;W64,X56,""))</f>
-        <v/>
+        <v>Kentucky</v>
       </c>
       <c r="W60" s="27"/>
       <c r="X60" s="156" t="str">
@@ -7437,7 +7485,9 @@
         <f>IF(F62&gt;F66,E62,IF(F66&gt;F62,E66,""))</f>
         <v>Arizona</v>
       </c>
-      <c r="H64" s="149"/>
+      <c r="H64" s="149">
+        <v>71</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="6"/>
       <c r="L64" s="2"/>
@@ -7451,7 +7501,9 @@
       <c r="T64" s="1"/>
       <c r="U64" s="6"/>
       <c r="V64" s="1"/>
-      <c r="W64" s="159"/>
+      <c r="W64" s="159">
+        <v>2</v>
+      </c>
       <c r="X64" s="153" t="str">
         <f>IF(Y66&gt;Y62,Z66,IF(Y62&gt;Y66,Z62,""))</f>
         <v>Kentucky</v>
@@ -8047,7 +8099,7 @@
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <selection pane="bottomRight" activeCell="X62" sqref="X62"/>
+      <selection pane="bottomRight" activeCell="V70" sqref="V70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8088,21 +8140,21 @@
       </c>
       <c r="J1" s="174">
         <f>J10+L10</f>
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="K1" s="174"/>
       <c r="L1" s="174"/>
       <c r="M1" s="174"/>
       <c r="N1" s="174">
         <f>N10+P10</f>
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="O1" s="174"/>
       <c r="P1" s="174"/>
       <c r="Q1" s="174"/>
       <c r="R1" s="174">
         <f>R10+T10</f>
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="S1" s="174"/>
       <c r="T1" s="174"/>
@@ -8304,7 +8356,7 @@
       </c>
       <c r="H5" s="6" t="str">
         <f>IF(COUNTBLANK(I45:I60)=0,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I5" s="6">
         <f>16*G44+SUM(D45:D60)</f>
@@ -8312,51 +8364,51 @@
       </c>
       <c r="J5" s="9">
         <f>SUM(K45:K60)</f>
-        <v>18</v>
-      </c>
-      <c r="K5" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="K5" s="10">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.625</v>
       </c>
       <c r="L5" s="9">
         <f>SUM(M45:M60)</f>
-        <v>20</v>
-      </c>
-      <c r="M5" s="10" t="str">
+        <v>22</v>
+      </c>
+      <c r="M5" s="10">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.6875</v>
       </c>
       <c r="N5" s="9">
         <f>SUM(O45:O60)</f>
-        <v>16</v>
-      </c>
-      <c r="O5" s="10" t="str">
+        <v>18</v>
+      </c>
+      <c r="O5" s="10">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.5625</v>
       </c>
       <c r="P5" s="9">
         <f>SUM(Q45:Q60)</f>
-        <v>16</v>
-      </c>
-      <c r="Q5" s="10" t="str">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0.5625</v>
       </c>
       <c r="R5" s="9">
         <f>SUM(S45:S60)</f>
-        <v>18</v>
-      </c>
-      <c r="S5" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="S5" s="10">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0.625</v>
       </c>
       <c r="T5" s="9">
         <f>SUM(U45:U60)</f>
-        <v>18</v>
-      </c>
-      <c r="U5" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="U5" s="10">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.625</v>
       </c>
       <c r="AH5" s="7" t="str">
         <f>Bracket!C10</f>
@@ -8375,7 +8427,7 @@
       </c>
       <c r="H6" s="6" t="str">
         <f>IF(COUNTBLANK(I62:I69)=0,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I6" s="6">
         <f>8*G61+SUM(D62:D69)</f>
@@ -8383,51 +8435,51 @@
       </c>
       <c r="J6" s="9">
         <f>SUM(K62:K69)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="K6" s="10">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.625</v>
       </c>
       <c r="L6" s="9">
         <f>SUM(M62:M69)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="10" t="str">
+        <v>20</v>
+      </c>
+      <c r="M6" s="10">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.625</v>
       </c>
       <c r="N6" s="9">
         <f>SUM(O62:O69)</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="10" t="str">
+        <v>16</v>
+      </c>
+      <c r="O6" s="10">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="P6" s="9">
         <f>SUM(Q62:Q69)</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="10" t="str">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0.375</v>
       </c>
       <c r="R6" s="9">
         <f>SUM(S62:S69)</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="10" t="str">
+        <v>12</v>
+      </c>
+      <c r="S6" s="10">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0.375</v>
       </c>
       <c r="T6" s="9">
         <f>SUM(U62:U69)</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="10" t="str">
+        <v>16</v>
+      </c>
+      <c r="U6" s="10">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="W6" s="11"/>
       <c r="X6" s="12"/>
@@ -8454,7 +8506,7 @@
       </c>
       <c r="H7" s="6" t="str">
         <f>IF(COUNTBLANK(I71:I74)=0,"Yes","No")</f>
-        <v>No</v>
+        <v>Yes</v>
       </c>
       <c r="I7" s="6">
         <f>4*G70+SUM(D71:D74)</f>
@@ -8462,51 +8514,51 @@
       </c>
       <c r="J7" s="9">
         <f>SUM(K71:K74)</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="K7" s="10">
         <f t="shared" si="0"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="L7" s="9">
         <f>SUM(M71:M74)</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="M7" s="10">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="N7" s="9">
         <f>SUM(O71:O74)</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="10" t="str">
+        <v>16</v>
+      </c>
+      <c r="O7" s="10">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="P7" s="9">
         <f>SUM(Q71:Q74)</f>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="Q7" s="10">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="R7" s="9">
         <f>SUM(S71:S74)</f>
-        <v>0</v>
-      </c>
-      <c r="S7" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="S7" s="10">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="T7" s="9">
         <f>SUM(U71:U74)</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="10" t="str">
+        <v>8</v>
+      </c>
+      <c r="U7" s="10">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.25</v>
       </c>
       <c r="W7" s="14"/>
       <c r="X7" s="102" t="s">
@@ -8691,7 +8743,7 @@
       </c>
       <c r="J10" s="9">
         <f>SUM(J4:J9)</f>
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="K10" s="10" t="str">
         <f>IF($H9="Yes",J10/$I10,"")</f>
@@ -8699,7 +8751,7 @@
       </c>
       <c r="L10" s="9">
         <f>SUM(L4:L9)</f>
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="M10" s="10" t="str">
         <f>IF($H9="Yes",L10/$I10,"")</f>
@@ -8707,7 +8759,7 @@
       </c>
       <c r="N10" s="9">
         <f>SUM(N4:N9)</f>
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="O10" s="10" t="str">
         <f>IF($H9="Yes",N10/$I10,"")</f>
@@ -8715,7 +8767,7 @@
       </c>
       <c r="P10" s="9">
         <f>SUM(P4:P9)</f>
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="10" t="str">
         <f>IF($H9="Yes",P10/$I10,"")</f>
@@ -8723,7 +8775,7 @@
       </c>
       <c r="R10" s="9">
         <f>SUM(R4:R9)</f>
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="S10" s="10" t="str">
         <f>IF($H9="Yes",R10/$I10,"")</f>
@@ -8731,7 +8783,7 @@
       </c>
       <c r="T10" s="9">
         <f>SUM(T4:T9)</f>
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="U10" s="10" t="str">
         <f>IF($H9="Yes",T10/$I10,"")</f>
@@ -13360,7 +13412,7 @@
       </c>
       <c r="C59" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Cincinnati</v>
       </c>
       <c r="D59" s="7">
         <f t="shared" si="18"/>
@@ -13382,49 +13434,49 @@
       </c>
       <c r="I59" s="68" t="str">
         <f>Bracket!X56</f>
-        <v/>
+        <v>UCLA</v>
       </c>
       <c r="J59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="K59" s="17">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="M59" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="O59" s="17">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="Q59" s="17">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="S59" s="17">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T59" s="69" t="s">
         <v>14</v>
       </c>
       <c r="U59" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH59" s="7" t="str">
         <f>Bracket!AB52</f>
@@ -13595,7 +13647,7 @@
       </c>
       <c r="C62" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Wisconsin</v>
       </c>
       <c r="D62" s="7">
         <f t="shared" ref="D62:D69" si="27">IF(SeedType=1,0,IF(SeedType=2,VLOOKUP(I62,SeedInfo,2,FALSE)*3,MAX(VLOOKUP(I62,SeedInfo,2,FALSE)-VLOOKUP(C62,SeedInfo,2,FALSE),0)))</f>
@@ -13617,7 +13669,7 @@
       </c>
       <c r="I62" s="68" t="str">
         <f>Bracket!I12</f>
-        <v/>
+        <v>Florida</v>
       </c>
       <c r="J62" s="139" t="s">
         <v>125</v>
@@ -13626,12 +13678,12 @@
         <f t="shared" ref="K62:K69" si="28">IF(J62&lt;&gt;"",IF($I62=J62,$G$61+$D62,0),"")</f>
         <v>0</v>
       </c>
-      <c r="L62" s="137" t="s">
+      <c r="L62" s="142" t="s">
         <v>77</v>
       </c>
       <c r="M62" s="17">
         <f t="shared" ref="M62:M69" si="29">IF(L62&lt;&gt;"",IF($I62=L62,$G$61+$D62,0),"")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N62" s="139" t="s">
         <v>125</v>
@@ -13681,7 +13733,7 @@
       </c>
       <c r="C63" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Baylor</v>
       </c>
       <c r="D63" s="7">
         <f t="shared" si="27"/>
@@ -13703,7 +13755,7 @@
       </c>
       <c r="I63" s="68" t="str">
         <f>Bracket!I28</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="J63" s="139" t="s">
         <v>98</v>
@@ -13756,7 +13808,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="str">
         <f t="shared" si="34"/>
         <v>Gonzaga</v>
@@ -13767,7 +13819,7 @@
       </c>
       <c r="C64" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>West Virginia</v>
       </c>
       <c r="D64" s="7">
         <f t="shared" si="27"/>
@@ -13789,16 +13841,16 @@
       </c>
       <c r="I64" s="68" t="str">
         <f>Bracket!I44</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="J64" s="69" t="s">
         <v>60</v>
       </c>
       <c r="K64" s="17">
         <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="L64" s="137" t="s">
+        <v>4</v>
+      </c>
+      <c r="L64" s="139" t="s">
         <v>259</v>
       </c>
       <c r="M64" s="17">
@@ -13810,28 +13862,28 @@
       </c>
       <c r="O64" s="17">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P64" s="69" t="s">
         <v>60</v>
       </c>
       <c r="Q64" s="17">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R64" s="69" t="s">
         <v>60</v>
       </c>
       <c r="S64" s="17">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T64" s="69" t="s">
         <v>60</v>
       </c>
       <c r="U64" s="17">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH64" s="7" t="str">
         <f>Bracket!AB62</f>
@@ -13853,7 +13905,7 @@
       </c>
       <c r="C65" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Arizona</v>
       </c>
       <c r="D65" s="7">
         <f t="shared" si="27"/>
@@ -13875,7 +13927,7 @@
       </c>
       <c r="I65" s="68" t="str">
         <f>Bracket!I60</f>
-        <v/>
+        <v>Xavier</v>
       </c>
       <c r="J65" s="69" t="s">
         <v>143</v>
@@ -13939,7 +13991,7 @@
       </c>
       <c r="C66" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Purdue</v>
       </c>
       <c r="D66" s="7">
         <f t="shared" si="27"/>
@@ -13961,49 +14013,49 @@
       </c>
       <c r="I66" s="68" t="str">
         <f>Bracket!V12</f>
-        <v/>
+        <v>Kansas</v>
       </c>
       <c r="J66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="K66" s="17">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="M66" s="17">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="O66" s="17">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="Q66" s="17">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="S66" s="17">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T66" s="69" t="s">
         <v>109</v>
       </c>
       <c r="U66" s="17">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH66" s="7" t="str">
         <f>Bracket!AB66</f>
@@ -14025,7 +14077,7 @@
       </c>
       <c r="C67" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Michigan</v>
       </c>
       <c r="D67" s="7">
         <f t="shared" si="27"/>
@@ -14047,28 +14099,28 @@
       </c>
       <c r="I67" s="68" t="str">
         <f>Bracket!V28</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="J67" s="69" t="s">
         <v>119</v>
       </c>
       <c r="K67" s="17">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L67" s="69" t="s">
         <v>119</v>
       </c>
       <c r="M67" s="17">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N67" s="69" t="s">
         <v>119</v>
       </c>
       <c r="O67" s="17">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P67" s="139" t="s">
         <v>72</v>
@@ -14082,14 +14134,14 @@
       </c>
       <c r="S67" s="17">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T67" s="69" t="s">
         <v>119</v>
       </c>
       <c r="U67" s="17">
         <f t="shared" si="33"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH67" s="7" t="str">
         <f>Bracket!AB68</f>
@@ -14111,7 +14163,7 @@
       </c>
       <c r="C68" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Butler</v>
       </c>
       <c r="D68" s="7">
         <f t="shared" si="27"/>
@@ -14133,35 +14185,35 @@
       </c>
       <c r="I68" s="68" t="str">
         <f>Bracket!V44</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="J68" s="69" t="s">
         <v>124</v>
       </c>
       <c r="K68" s="17">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L68" s="69" t="s">
         <v>124</v>
       </c>
       <c r="M68" s="17">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N68" s="69" t="s">
         <v>124</v>
       </c>
       <c r="O68" s="17">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P68" s="69" t="s">
         <v>124</v>
       </c>
       <c r="Q68" s="17">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R68" s="69" t="s">
         <v>135</v>
@@ -14175,13 +14227,13 @@
       </c>
       <c r="U68" s="17">
         <f t="shared" si="33"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="str">
         <f t="shared" si="34"/>
-        <v/>
+        <v>UCLA</v>
       </c>
       <c r="B69" s="7" t="str">
         <f t="shared" si="35"/>
@@ -14189,7 +14241,7 @@
       </c>
       <c r="C69" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>UCLA</v>
       </c>
       <c r="D69" s="7">
         <f t="shared" si="27"/>
@@ -14197,7 +14249,7 @@
       </c>
       <c r="E69" s="72" t="str">
         <f>Bracket!X56</f>
-        <v/>
+        <v>UCLA</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>21</v>
@@ -14211,21 +14263,21 @@
       </c>
       <c r="I69" s="68" t="str">
         <f>Bracket!V60</f>
-        <v/>
-      </c>
-      <c r="J69" s="137" t="s">
+        <v>Kentucky</v>
+      </c>
+      <c r="J69" s="142" t="s">
         <v>84</v>
       </c>
       <c r="K69" s="17">
         <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="L69" s="137" t="s">
+        <v>4</v>
+      </c>
+      <c r="L69" s="142" t="s">
         <v>84</v>
       </c>
       <c r="M69" s="17">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N69" s="69" t="s">
         <v>14</v>
@@ -14314,15 +14366,15 @@
     <row r="71" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="str">
         <f>E71</f>
-        <v/>
+        <v>Florida</v>
       </c>
       <c r="B71" s="7" t="str">
         <f>G71</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="C71" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Florida</v>
       </c>
       <c r="D71" s="7">
         <f>IF(SeedType=1,0,IF(SeedType=2,VLOOKUP(I71,SeedInfo,2,FALSE)*4,MAX(VLOOKUP(I71,SeedInfo,2,FALSE)-VLOOKUP(C71,SeedInfo,2,FALSE),0)))</f>
@@ -14330,21 +14382,21 @@
       </c>
       <c r="E71" s="72" t="str">
         <f>Bracket!I12</f>
-        <v/>
+        <v>Florida</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G71" s="72" t="str">
         <f>Bracket!I28</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="H71" s="6">
         <v>57</v>
       </c>
       <c r="I71" s="68" t="str">
         <f>Bracket!K20</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="J71" s="139" t="s">
         <v>98</v>
@@ -14389,18 +14441,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="str">
         <f>E72</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="B72" s="7" t="str">
         <f>G72</f>
-        <v/>
+        <v>Xavier</v>
       </c>
       <c r="C72" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Xavier</v>
       </c>
       <c r="D72" s="7">
         <f>IF(SeedType=1,0,IF(SeedType=2,VLOOKUP(I72,SeedInfo,2,FALSE)*4,MAX(VLOOKUP(I72,SeedInfo,2,FALSE)-VLOOKUP(C72,SeedInfo,2,FALSE),0)))</f>
@@ -14408,37 +14460,37 @@
       </c>
       <c r="E72" s="72" t="str">
         <f>Bracket!I44</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G72" s="72" t="str">
         <f>Bracket!I60</f>
-        <v/>
+        <v>Xavier</v>
       </c>
       <c r="H72" s="6">
         <v>58</v>
       </c>
       <c r="I72" s="68" t="str">
         <f>Bracket!K52</f>
-        <v/>
-      </c>
-      <c r="J72" s="69" t="s">
+        <v>Gonzaga</v>
+      </c>
+      <c r="J72" s="139" t="s">
         <v>143</v>
       </c>
       <c r="K72" s="17">
         <f>IF(J72&lt;&gt;"",IF($I72=J72,$G$70+$D72,0),"")</f>
         <v>0</v>
       </c>
-      <c r="L72" s="69" t="s">
+      <c r="L72" s="139" t="s">
         <v>143</v>
       </c>
       <c r="M72" s="17">
         <f>IF(L72&lt;&gt;"",IF($I72=L72,$G$70+$D72,0),"")</f>
         <v>0</v>
       </c>
-      <c r="N72" s="69" t="s">
+      <c r="N72" s="139" t="s">
         <v>143</v>
       </c>
       <c r="O72" s="17">
@@ -14450,16 +14502,16 @@
       </c>
       <c r="Q72" s="17">
         <f>IF(P72&lt;&gt;"",IF($I72=P72,$G$70+$D72,0),"")</f>
-        <v>0</v>
-      </c>
-      <c r="R72" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="R72" s="139" t="s">
         <v>143</v>
       </c>
       <c r="S72" s="17">
         <f>IF(R72&lt;&gt;"",IF($I72=R72,$G$70+$D72,0),"")</f>
         <v>0</v>
       </c>
-      <c r="T72" s="69" t="s">
+      <c r="T72" s="139" t="s">
         <v>143</v>
       </c>
       <c r="U72" s="17">
@@ -14470,15 +14522,15 @@
     <row r="73" spans="1:35" x14ac:dyDescent="0.15">
       <c r="A73" s="7" t="str">
         <f>E73</f>
-        <v/>
+        <v>Kansas</v>
       </c>
       <c r="B73" s="7" t="str">
         <f>G73</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="C73" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Kansas</v>
       </c>
       <c r="D73" s="7">
         <f>IF(SeedType=1,0,IF(SeedType=2,VLOOKUP(I73,SeedInfo,2,FALSE)*4,MAX(VLOOKUP(I73,SeedInfo,2,FALSE)-VLOOKUP(C73,SeedInfo,2,FALSE),0)))</f>
@@ -14486,21 +14538,21 @@
       </c>
       <c r="E73" s="72" t="str">
         <f>Bracket!V12</f>
-        <v/>
+        <v>Kansas</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G73" s="72" t="str">
         <f>Bracket!V28</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="H73" s="6">
         <v>59</v>
       </c>
       <c r="I73" s="68" t="str">
         <f>Bracket!T20</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="J73" s="137" t="s">
         <v>109</v>
@@ -14521,7 +14573,7 @@
       </c>
       <c r="O73" s="17">
         <f>IF(N73&lt;&gt;"",IF($I73=N73,$G$70+$D73,0),"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="P73" s="69" t="s">
         <v>109</v>
@@ -14535,28 +14587,28 @@
       </c>
       <c r="S73" s="17">
         <f>IF(R73&lt;&gt;"",IF($I73=R73,$G$70+$D73,0),"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T73" s="69" t="s">
         <v>119</v>
       </c>
       <c r="U73" s="17">
         <f>IF(T73&lt;&gt;"",IF($I73=T73,$G$70+$D73,0),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="str">
         <f>E74</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="B74" s="7" t="str">
         <f>G74</f>
-        <v/>
+        <v>Kentucky</v>
       </c>
       <c r="C74" s="7" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>Kentucky</v>
       </c>
       <c r="D74" s="7">
         <f>IF(SeedType=1,0,IF(SeedType=2,VLOOKUP(I74,SeedInfo,2,FALSE)*4,MAX(VLOOKUP(I74,SeedInfo,2,FALSE)-VLOOKUP(C74,SeedInfo,2,FALSE),0)))</f>
@@ -14564,58 +14616,58 @@
       </c>
       <c r="E74" s="72" t="str">
         <f>Bracket!V44</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G74" s="72" t="str">
         <f>Bracket!V60</f>
-        <v/>
+        <v>Kentucky</v>
       </c>
       <c r="H74" s="6">
         <v>60</v>
       </c>
       <c r="I74" s="68" t="str">
         <f>Bracket!T52</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="J74" s="137" t="s">
         <v>124</v>
       </c>
       <c r="K74" s="17">
         <f>IF(J74&lt;&gt;"",IF($I74=J74,$G$70+$D74,0),"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L74" s="137" t="s">
         <v>124</v>
       </c>
       <c r="M74" s="17">
         <f>IF(L74&lt;&gt;"",IF($I74=L74,$G$70+$D74,0),"")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N74" s="69" t="s">
         <v>124</v>
       </c>
       <c r="O74" s="17">
         <f>IF(N74&lt;&gt;"",IF($I74=N74,$G$70+$D74,0),"")</f>
-        <v>0</v>
-      </c>
-      <c r="P74" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="P74" s="139" t="s">
         <v>14</v>
       </c>
       <c r="Q74" s="17">
         <f>IF(P74&lt;&gt;"",IF($I74=P74,$G$70+$D74,0),"")</f>
         <v>0</v>
       </c>
-      <c r="R74" s="69" t="s">
+      <c r="R74" s="139" t="s">
         <v>14</v>
       </c>
       <c r="S74" s="17">
         <f>IF(R74&lt;&gt;"",IF($I74=R74,$G$70+$D74,0),"")</f>
         <v>0</v>
       </c>
-      <c r="T74" s="69" t="s">
+      <c r="T74" s="139" t="s">
         <v>14</v>
       </c>
       <c r="U74" s="17">
@@ -14681,11 +14733,11 @@
     <row r="76" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="str">
         <f>E76</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="B76" s="7" t="str">
         <f>G76</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="C76" s="7" t="str">
         <f t="shared" si="15"/>
@@ -14697,14 +14749,14 @@
       </c>
       <c r="E76" s="72" t="str">
         <f>Bracket!K20</f>
-        <v/>
+        <v>South Carolina</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G76" s="72" t="str">
         <f>Bracket!K52</f>
-        <v/>
+        <v>Gonzaga</v>
       </c>
       <c r="H76" s="6">
         <v>61</v>
@@ -14720,14 +14772,14 @@
         <f>IF(J76&lt;&gt;"",IF($I76=J76,$G$75+$D76,0),"")</f>
         <v>0</v>
       </c>
-      <c r="L76" s="69" t="s">
+      <c r="L76" s="139" t="s">
         <v>143</v>
       </c>
       <c r="M76" s="17">
         <f>IF(L76&lt;&gt;"",IF($I76=L76,$G$75+$D76,0),"")</f>
         <v>0</v>
       </c>
-      <c r="N76" s="69" t="s">
+      <c r="N76" s="139" t="s">
         <v>143</v>
       </c>
       <c r="O76" s="17">
@@ -14741,14 +14793,14 @@
         <f>IF(P76&lt;&gt;"",IF($I76=P76,$G$75+$D76,0),"")</f>
         <v>0</v>
       </c>
-      <c r="R76" s="69" t="s">
+      <c r="R76" s="139" t="s">
         <v>143</v>
       </c>
       <c r="S76" s="17">
         <f>IF(R76&lt;&gt;"",IF($I76=R76,$G$75+$D76,0),"")</f>
         <v>0</v>
       </c>
-      <c r="T76" s="69" t="s">
+      <c r="T76" s="139" t="s">
         <v>143</v>
       </c>
       <c r="U76" s="17">
@@ -14756,14 +14808,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="str">
         <f>E77</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="B77" s="7" t="str">
         <f>G77</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="C77" s="7" t="str">
         <f>IF(I77="","",IF(A77=I77,B77,A77))</f>
@@ -14775,14 +14827,14 @@
       </c>
       <c r="E77" s="72" t="str">
         <f>Bracket!T20</f>
-        <v/>
+        <v>Oregon</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G77" s="72" t="str">
         <f>Bracket!T52</f>
-        <v/>
+        <v>North Carolina</v>
       </c>
       <c r="H77" s="6">
         <v>62</v>
@@ -14791,7 +14843,7 @@
         <f>Bracket!P40</f>
         <v/>
       </c>
-      <c r="J77" s="69" t="s">
+      <c r="J77" s="139" t="s">
         <v>109</v>
       </c>
       <c r="K77" s="17">
@@ -14812,21 +14864,21 @@
         <f>IF(N77&lt;&gt;"",IF($I77=N77,$G$75+$D77,0),"")</f>
         <v>0</v>
       </c>
-      <c r="P77" s="137" t="s">
+      <c r="P77" s="139" t="s">
         <v>14</v>
       </c>
       <c r="Q77" s="17">
         <f>IF(P77&lt;&gt;"",IF($I77=P77,$G$75+$D77,0),"")</f>
         <v>0</v>
       </c>
-      <c r="R77" s="69" t="s">
+      <c r="R77" s="139" t="s">
         <v>14</v>
       </c>
       <c r="S77" s="17">
         <f>IF(R77&lt;&gt;"",IF($I77=R77,$G$75+$D77,0),"")</f>
         <v>0</v>
       </c>
-      <c r="T77" s="69" t="s">
+      <c r="T77" s="139" t="s">
         <v>14</v>
       </c>
       <c r="U77" s="17">
@@ -14893,7 +14945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:35" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="str">
         <f>E79</f>
         <v/>
@@ -14928,7 +14980,7 @@
         <f>Bracket!N33</f>
         <v/>
       </c>
-      <c r="J79" s="69" t="s">
+      <c r="J79" s="139" t="s">
         <v>109</v>
       </c>
       <c r="K79" s="17">
@@ -14956,14 +15008,14 @@
         <f>IF(P79&lt;&gt;"",IF($I79=P79,$G$78+$D79,0),"")</f>
         <v>0</v>
       </c>
-      <c r="R79" s="137" t="s">
+      <c r="R79" s="139" t="s">
         <v>143</v>
       </c>
       <c r="S79" s="17">
         <f>IF(R79&lt;&gt;"",IF($I79=R79,$G$78+$D79,0),"")</f>
         <v>0</v>
       </c>
-      <c r="T79" s="69" t="s">
+      <c r="T79" s="139" t="s">
         <v>143</v>
       </c>
       <c r="U79" s="17">

</xml_diff>